<commit_message>
Popeye: 修改100pin excel中中断配置的几个Interrupt function name.
</commit_message>
<xml_diff>
--- a/Pin100.xlsx
+++ b/Pin100.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\McuCode\GEN_RH850_F1L\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="14970" windowHeight="7515"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="14970" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pinmux配置" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pinmux配置!$A$1:$P$301</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -29,7 +24,7 @@
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -254,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -346,7 +341,7 @@
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -398,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -455,7 +450,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="872">
   <si>
     <t>Pin</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3193,218 +3188,212 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ISR_TAUD0I1func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_TAUD0I5func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I7func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I9func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I11func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I13func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I15func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I3func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_IIC0RIfunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_IIC0TIfunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_IIC0TEIfunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_IIC0EEfunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_TAUJ0I2func</t>
+  </si>
+  <si>
+    <t>ISR_TAUJ0I3func</t>
+  </si>
+  <si>
+    <t>ISR_TAUJ0I0func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_TAUJ0I1func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_OSTM0func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_PWGA2func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA3func</t>
+  </si>
+  <si>
+    <t>ISR_DMA0func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_DMA1func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_DMA2func</t>
+  </si>
+  <si>
+    <t>ISR_DMA3func</t>
+  </si>
+  <si>
+    <t>ISR_DMA4func</t>
+  </si>
+  <si>
+    <t>ISR_DMA5func</t>
+  </si>
+  <si>
+    <t>ISR_DMA6func</t>
+  </si>
+  <si>
+    <t>ISR_DMA7func</t>
+  </si>
+  <si>
+    <t>ISR_DMA8func</t>
+  </si>
+  <si>
+    <t>ISR_DMA9func</t>
+  </si>
+  <si>
+    <t>ISR_DMA10func</t>
+  </si>
+  <si>
+    <t>ISR_DMA11func</t>
+  </si>
+  <si>
+    <t>ISR_DMA12func</t>
+  </si>
+  <si>
+    <t>ISR_DMA13func</t>
+  </si>
+  <si>
+    <t>ISR_DMA14func</t>
+  </si>
+  <si>
+    <t>ISR_DMA15func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA0func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_PWGA4func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA5func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA1func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_PWGA6func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA7func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA8func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA9func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA10func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA11func</t>
+  </si>
+  <si>
+    <t>ISR_TAUD0I12func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanIsrStatus_1func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanIsrTx_1func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSIH1_Rx_handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSIH1_Tx_handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSIH1_Error_handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART1_Tx_Handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART1_Rx_Handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART1_Error_Handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_PWGA20func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_PWGA22func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA23func</t>
+  </si>
+  <si>
+    <t>ISR_INTP8func</t>
+  </si>
+  <si>
+    <t>ISR_PWGA21func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ISR_INTP6func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ISR_INTP7func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I1func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_TAUD0I5func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I7func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I9func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I11func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I13func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I15func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I3func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_IIC0RIfunc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_IIC0TIfunc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_IIC0TEIfunc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_IIC0EEfunc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_TAUJ0I2func</t>
-  </si>
-  <si>
-    <t>ISR_TAUJ0I3func</t>
-  </si>
-  <si>
-    <t>ISR_TAUJ0I0func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_TAUJ0I1func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_OSTM0func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_PWGA2func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA3func</t>
-  </si>
-  <si>
-    <t>ISR_DMA0func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_DMA1func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_DMA2func</t>
-  </si>
-  <si>
-    <t>ISR_DMA3func</t>
-  </si>
-  <si>
-    <t>ISR_DMA4func</t>
-  </si>
-  <si>
-    <t>ISR_DMA5func</t>
-  </si>
-  <si>
-    <t>ISR_DMA6func</t>
-  </si>
-  <si>
-    <t>ISR_DMA7func</t>
-  </si>
-  <si>
-    <t>ISR_DMA8func</t>
-  </si>
-  <si>
-    <t>ISR_DMA9func</t>
-  </si>
-  <si>
-    <t>ISR_DMA10func</t>
-  </si>
-  <si>
-    <t>ISR_DMA11func</t>
-  </si>
-  <si>
-    <t>ISR_DMA12func</t>
-  </si>
-  <si>
-    <t>ISR_DMA13func</t>
-  </si>
-  <si>
-    <t>ISR_DMA14func</t>
-  </si>
-  <si>
-    <t>ISR_DMA15func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA0func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_PWGA4func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA5func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA1func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_PWGA6func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA7func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA8func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA9func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA10func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA11func</t>
-  </si>
-  <si>
-    <t>ISR_TAUD0I12func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CanIsrStatus_1func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CanIsrTx_1func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSIH1_Rx_handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSIH1_Tx_handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSIH1_Error_handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UART1_Tx_Handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UART1_Rx_Handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UART1_Error_Handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_PWGA20func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_PWGA22func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA23func</t>
-  </si>
-  <si>
-    <t>ISR_INTP8func</t>
-  </si>
-  <si>
-    <t>ISR_PWGA21func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_INTP6func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISR_INTP7func</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3586,6 +3575,26 @@
   </si>
   <si>
     <t>CanIsrTx_2func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_INTP10func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISR_INTP11func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART3_Tx_Handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART3_Rx_Handler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART3_Error_Handler</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4540,40 +4549,10 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4604,6 +4583,108 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4650,78 +4731,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4789,7 +4798,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4831,7 +4840,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4866,7 +4875,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5077,8 +5086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -5154,11 +5163,11 @@
       <c r="P1" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="R1" s="77" t="s">
+      <c r="R1" s="67" t="s">
         <v>563</v>
       </c>
-      <c r="S1" s="78"/>
-      <c r="T1" s="79"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="69"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A2" s="37">
@@ -5209,9 +5218,9 @@
       <c r="P2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="82"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A3" s="24">
@@ -5247,10 +5256,10 @@
       <c r="R3" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="S3" s="83" t="s">
+      <c r="S3" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="84"/>
+      <c r="T3" s="74"/>
     </row>
     <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A4" s="24">
@@ -5283,7 +5292,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="39"/>
-      <c r="R4" s="67" t="s">
+      <c r="R4" s="63" t="s">
         <v>137</v>
       </c>
       <c r="S4" s="12" t="s">
@@ -5326,7 +5335,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="39"/>
-      <c r="R5" s="67"/>
+      <c r="R5" s="63"/>
       <c r="S5" s="12" t="s">
         <v>139</v>
       </c>
@@ -5370,10 +5379,10 @@
       <c r="R6" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="S6" s="75" t="s">
+      <c r="S6" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="T6" s="76"/>
+      <c r="T6" s="66"/>
     </row>
     <row r="7" spans="1:20" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A7" s="24">
@@ -5427,10 +5436,10 @@
       <c r="R7" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="S7" s="75" t="s">
+      <c r="S7" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="T7" s="76"/>
+      <c r="T7" s="66"/>
     </row>
     <row r="8" spans="1:20" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A8" s="24">
@@ -5484,10 +5493,10 @@
       <c r="R8" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="S8" s="75" t="s">
+      <c r="S8" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="T8" s="76"/>
+      <c r="T8" s="66"/>
     </row>
     <row r="9" spans="1:20" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A9" s="24">
@@ -5525,10 +5534,10 @@
       <c r="R9" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="S9" s="75" t="s">
+      <c r="S9" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="T9" s="76"/>
+      <c r="T9" s="66"/>
     </row>
     <row r="10" spans="1:20" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="24">
@@ -5559,7 +5568,7 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="39"/>
-      <c r="R10" s="67" t="s">
+      <c r="R10" s="63" t="s">
         <v>149</v>
       </c>
       <c r="S10" s="12" t="s">
@@ -5618,7 +5627,7 @@
       <c r="P11" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="R11" s="67"/>
+      <c r="R11" s="63"/>
       <c r="S11" s="12" t="s">
         <v>151</v>
       </c>
@@ -5662,10 +5671,10 @@
       <c r="R12" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="S12" s="75" t="s">
+      <c r="S12" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="T12" s="76"/>
+      <c r="T12" s="66"/>
     </row>
     <row r="13" spans="1:20" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A13" s="24">
@@ -5784,7 +5793,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="39"/>
-      <c r="R15" s="67" t="s">
+      <c r="R15" s="63" t="s">
         <v>160</v>
       </c>
       <c r="S15" s="12" t="s">
@@ -5825,7 +5834,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="39"/>
-      <c r="R16" s="67"/>
+      <c r="R16" s="63"/>
       <c r="S16" s="12" t="s">
         <v>163</v>
       </c>
@@ -5866,7 +5875,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="39"/>
-      <c r="R17" s="67" t="s">
+      <c r="R17" s="63" t="s">
         <v>165</v>
       </c>
       <c r="S17" s="12" t="s">
@@ -5905,7 +5914,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="39"/>
-      <c r="R18" s="67"/>
+      <c r="R18" s="63"/>
       <c r="S18" s="12" t="s">
         <v>163</v>
       </c>
@@ -5962,7 +5971,7 @@
       <c r="P19" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="R19" s="67" t="s">
+      <c r="R19" s="63" t="s">
         <v>168</v>
       </c>
       <c r="S19" s="12" t="s">
@@ -6003,7 +6012,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="39"/>
-      <c r="R20" s="67"/>
+      <c r="R20" s="63"/>
       <c r="S20" s="12" t="s">
         <v>163</v>
       </c>
@@ -6040,7 +6049,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="39"/>
-      <c r="R21" s="67" t="s">
+      <c r="R21" s="63" t="s">
         <v>172</v>
       </c>
       <c r="S21" s="12" t="s">
@@ -6079,7 +6088,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="39"/>
-      <c r="R22" s="63"/>
+      <c r="R22" s="64"/>
       <c r="S22" s="13" t="s">
         <v>163</v>
       </c>
@@ -6116,10 +6125,10 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="39"/>
-      <c r="R23" s="63" t="s">
+      <c r="R23" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="S23" s="66" t="s">
+      <c r="S23" s="77" t="s">
         <v>161</v>
       </c>
       <c r="T23" s="51" t="s">
@@ -6155,8 +6164,8 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="39"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="66"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="77"/>
       <c r="T24" s="52" t="s">
         <v>177</v>
       </c>
@@ -6190,8 +6199,8 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="39"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="66" t="s">
+      <c r="R25" s="75"/>
+      <c r="S25" s="77" t="s">
         <v>178</v>
       </c>
       <c r="T25" s="51" t="s">
@@ -6227,8 +6236,8 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="39"/>
-      <c r="R26" s="65"/>
-      <c r="S26" s="66"/>
+      <c r="R26" s="76"/>
+      <c r="S26" s="77"/>
       <c r="T26" s="52" t="s">
         <v>180</v>
       </c>
@@ -6262,7 +6271,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="39"/>
-      <c r="R27" s="67" t="s">
+      <c r="R27" s="63" t="s">
         <v>181</v>
       </c>
       <c r="S27" s="14" t="s">
@@ -6303,7 +6312,7 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="39"/>
-      <c r="R28" s="67"/>
+      <c r="R28" s="63"/>
       <c r="S28" s="14" t="s">
         <v>178</v>
       </c>
@@ -6340,7 +6349,7 @@
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="39"/>
-      <c r="R29" s="67" t="s">
+      <c r="R29" s="63" t="s">
         <v>185</v>
       </c>
       <c r="S29" s="14" t="s">
@@ -6399,7 +6408,7 @@
       <c r="P30" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="R30" s="74"/>
+      <c r="R30" s="84"/>
       <c r="S30" s="53" t="s">
         <v>178</v>
       </c>
@@ -6506,10 +6515,10 @@
       <c r="P32" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="R32" s="72" t="s">
+      <c r="R32" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="S32" s="73"/>
+      <c r="S32" s="83"/>
     </row>
     <row r="33" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A33" s="27">
@@ -6776,10 +6785,10 @@
       <c r="P37" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="R37" s="68" t="s">
+      <c r="R37" s="78" t="s">
         <v>565</v>
       </c>
-      <c r="S37" s="69"/>
+      <c r="S37" s="79"/>
     </row>
     <row r="38" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="24">
@@ -6810,8 +6819,8 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="39"/>
-      <c r="R38" s="70"/>
-      <c r="S38" s="71"/>
+      <c r="R38" s="80"/>
+      <c r="S38" s="81"/>
     </row>
     <row r="39" spans="1:19" ht="17.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A39" s="24">
@@ -15994,6 +16003,19 @@
   <sheetProtection algorithmName="SHA-512" hashValue="9iKcavKJ7bXa2VAXjnQktA7bMIa0L+ozlYV01ValeWFg/EGf+5wj1snCiPjUkrGoeuoMsiLxPW4Cunz4U5jV4A==" saltValue="ziT6rR81fzZhA4TygKZN8w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A1:P301"/>
   <mergeCells count="20">
+    <mergeCell ref="R23:R26"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="R27:R28"/>
+    <mergeCell ref="R37:S38"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="R29:R30"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="R1:T2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
     <mergeCell ref="R19:R20"/>
     <mergeCell ref="R21:R22"/>
     <mergeCell ref="S9:T9"/>
@@ -16001,19 +16023,6 @@
     <mergeCell ref="S12:T12"/>
     <mergeCell ref="R15:R16"/>
     <mergeCell ref="R17:R18"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="R1:T2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="R23:R26"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="R27:R28"/>
-    <mergeCell ref="R37:S38"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="R29:R30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="70">
@@ -16238,9 +16247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B213" sqref="B213"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -16273,12 +16282,12 @@
       <c r="F1" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="H1" s="85" t="s">
+      <c r="H1" s="109" t="s">
         <v>560</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="87"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="111"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="24">
@@ -16299,12 +16308,12 @@
       <c r="F2" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="112" t="s">
         <v>561</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="90"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24">
@@ -16325,12 +16334,12 @@
       <c r="F3" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="115" t="s">
         <v>562</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="93"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="117"/>
     </row>
     <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="24">
@@ -16351,12 +16360,12 @@
       <c r="F4" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="H4" s="94" t="s">
+      <c r="H4" s="118" t="s">
         <v>564</v>
       </c>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="96"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="120"/>
     </row>
     <row r="5" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
@@ -16377,10 +16386,10 @@
       <c r="F5" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="99"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="123"/>
     </row>
     <row r="6" spans="1:11" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A6" s="24">
@@ -16436,7 +16445,7 @@
         <v>575</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>397</v>
@@ -16469,11 +16478,11 @@
       <c r="B10" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="112" t="s">
+      <c r="C10" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D10" s="113"/>
-      <c r="E10" s="114"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90"/>
       <c r="F10" s="25" t="s">
         <v>399</v>
       </c>
@@ -16485,9 +16494,9 @@
       <c r="B11" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="C11" s="115"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="117"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="96"/>
       <c r="F11" s="25" t="s">
         <v>400</v>
       </c>
@@ -16559,11 +16568,11 @@
       <c r="B15" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="85" t="s">
         <v>583</v>
       </c>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="87"/>
       <c r="F15" s="26" t="s">
         <v>404</v>
       </c>
@@ -16673,11 +16682,11 @@
       <c r="B21" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="C21" s="112" t="s">
+      <c r="C21" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D21" s="113"/>
-      <c r="E21" s="114"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="90"/>
       <c r="F21" s="26" t="s">
         <v>410</v>
       </c>
@@ -16689,9 +16698,9 @@
       <c r="B22" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="117"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
       <c r="F22" s="26" t="s">
         <v>411</v>
       </c>
@@ -16757,11 +16766,11 @@
       <c r="B26" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C26" s="112" t="s">
+      <c r="C26" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D26" s="113"/>
-      <c r="E26" s="114"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="90"/>
       <c r="F26" s="26" t="s">
         <v>415</v>
       </c>
@@ -16773,9 +16782,9 @@
       <c r="B27" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="115"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="117"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
       <c r="F27" s="26" t="s">
         <v>416</v>
       </c>
@@ -16990,7 +16999,7 @@
         <v>603</v>
       </c>
       <c r="E39" s="60" t="s">
-        <v>752</v>
+        <v>867</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>421</v>
@@ -17008,7 +17017,7 @@
         <v>604</v>
       </c>
       <c r="E40" s="60" t="s">
-        <v>753</v>
+        <v>868</v>
       </c>
       <c r="F40" s="25" t="s">
         <v>421</v>
@@ -17028,7 +17037,7 @@
         <v>605</v>
       </c>
       <c r="E41" s="60" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="F41" s="25" t="s">
         <v>424</v>
@@ -17046,7 +17055,7 @@
         <v>606</v>
       </c>
       <c r="E42" s="60" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="F42" s="25" t="s">
         <v>425</v>
@@ -17064,7 +17073,7 @@
         <v>580</v>
       </c>
       <c r="E43" s="60" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F43" s="25" t="s">
         <v>426</v>
@@ -17082,7 +17091,7 @@
         <v>581</v>
       </c>
       <c r="E44" s="60" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F44" s="25" t="s">
         <v>427</v>
@@ -17100,7 +17109,7 @@
         <v>607</v>
       </c>
       <c r="E45" s="60" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F45" s="25" t="s">
         <v>428</v>
@@ -17120,7 +17129,7 @@
         <v>608</v>
       </c>
       <c r="E46" s="60" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F46" s="25" t="s">
         <v>429</v>
@@ -17138,7 +17147,7 @@
         <v>609</v>
       </c>
       <c r="E47" s="60" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="F47" s="25" t="s">
         <v>430</v>
@@ -17158,7 +17167,7 @@
         <v>610</v>
       </c>
       <c r="E48" s="60" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F48" s="25" t="s">
         <v>431</v>
@@ -17171,11 +17180,11 @@
       <c r="B49" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="C49" s="118" t="s">
+      <c r="C49" s="85" t="s">
         <v>583</v>
       </c>
-      <c r="D49" s="119"/>
-      <c r="E49" s="120"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="87"/>
       <c r="F49" s="25" t="s">
         <v>432</v>
       </c>
@@ -17184,13 +17193,13 @@
       <c r="A50" s="27">
         <v>48</v>
       </c>
-      <c r="B50" s="109" t="s">
+      <c r="B50" s="106" t="s">
         <v>433</v>
       </c>
-      <c r="C50" s="110"/>
-      <c r="D50" s="110"/>
-      <c r="E50" s="110"/>
-      <c r="F50" s="111"/>
+      <c r="C50" s="107"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="107"/>
+      <c r="F50" s="108"/>
     </row>
     <row r="51" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="24">
@@ -17199,11 +17208,11 @@
       <c r="B51" s="19" t="s">
         <v>375</v>
       </c>
-      <c r="C51" s="112" t="s">
+      <c r="C51" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D51" s="113"/>
-      <c r="E51" s="114"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="90"/>
       <c r="F51" s="25" t="s">
         <v>434</v>
       </c>
@@ -17215,9 +17224,9 @@
       <c r="B52" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="C52" s="121"/>
-      <c r="D52" s="122"/>
-      <c r="E52" s="123"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="92"/>
+      <c r="E52" s="93"/>
       <c r="F52" s="25" t="s">
         <v>435</v>
       </c>
@@ -17229,9 +17238,9 @@
       <c r="B53" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C53" s="115"/>
-      <c r="D53" s="116"/>
-      <c r="E53" s="117"/>
+      <c r="C53" s="94"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="96"/>
       <c r="F53" s="25" t="s">
         <v>436</v>
       </c>
@@ -17248,7 +17257,7 @@
         <v>611</v>
       </c>
       <c r="E54" s="60" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F54" s="25" t="s">
         <v>437</v>
@@ -17266,7 +17275,7 @@
         <v>620</v>
       </c>
       <c r="E55" s="60" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F55" s="25" t="s">
         <v>438</v>
@@ -17284,7 +17293,7 @@
         <v>612</v>
       </c>
       <c r="E56" s="60" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F56" s="25" t="s">
         <v>439</v>
@@ -17302,7 +17311,7 @@
         <v>613</v>
       </c>
       <c r="E57" s="60" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F57" s="25" t="s">
         <v>440</v>
@@ -17320,7 +17329,7 @@
         <v>614</v>
       </c>
       <c r="E58" s="60" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F58" s="25" t="s">
         <v>441</v>
@@ -17338,7 +17347,7 @@
         <v>615</v>
       </c>
       <c r="E59" s="60" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F59" s="25" t="s">
         <v>442</v>
@@ -17356,7 +17365,7 @@
         <v>616</v>
       </c>
       <c r="E60" s="60" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F60" s="25" t="s">
         <v>443</v>
@@ -17374,7 +17383,7 @@
         <v>617</v>
       </c>
       <c r="E61" s="60" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F61" s="25" t="s">
         <v>444</v>
@@ -17392,7 +17401,7 @@
         <v>618</v>
       </c>
       <c r="E62" s="60" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F62" s="25" t="s">
         <v>445</v>
@@ -17410,7 +17419,7 @@
         <v>619</v>
       </c>
       <c r="E63" s="60" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F63" s="25" t="s">
         <v>446</v>
@@ -17428,7 +17437,7 @@
         <v>621</v>
       </c>
       <c r="E64" s="60" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F64" s="25" t="s">
         <v>447</v>
@@ -17448,7 +17457,7 @@
         <v>622</v>
       </c>
       <c r="E65" s="60" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F65" s="25" t="s">
         <v>448</v>
@@ -17466,7 +17475,7 @@
         <v>623</v>
       </c>
       <c r="E66" s="60" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F66" s="25" t="s">
         <v>449</v>
@@ -17484,7 +17493,7 @@
         <v>624</v>
       </c>
       <c r="E67" s="60" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="F67" s="25" t="s">
         <v>450</v>
@@ -17502,7 +17511,7 @@
         <v>625</v>
       </c>
       <c r="E68" s="60" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F68" s="25" t="s">
         <v>451</v>
@@ -17520,7 +17529,7 @@
         <v>626</v>
       </c>
       <c r="E69" s="60" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F69" s="25" t="s">
         <v>452</v>
@@ -17538,7 +17547,7 @@
         <v>627</v>
       </c>
       <c r="E70" s="60" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="F70" s="25" t="s">
         <v>453</v>
@@ -17556,7 +17565,7 @@
         <v>628</v>
       </c>
       <c r="E71" s="60" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="F71" s="25" t="s">
         <v>454</v>
@@ -17574,7 +17583,7 @@
         <v>629</v>
       </c>
       <c r="E72" s="60" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F72" s="25" t="s">
         <v>455</v>
@@ -17592,7 +17601,7 @@
         <v>630</v>
       </c>
       <c r="E73" s="60" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F73" s="25" t="s">
         <v>456</v>
@@ -17610,7 +17619,7 @@
         <v>631</v>
       </c>
       <c r="E74" s="60" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="F74" s="25" t="s">
         <v>457</v>
@@ -17628,7 +17637,7 @@
         <v>632</v>
       </c>
       <c r="E75" s="60" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="F75" s="25" t="s">
         <v>458</v>
@@ -17646,7 +17655,7 @@
         <v>633</v>
       </c>
       <c r="E76" s="60" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="F76" s="25" t="s">
         <v>459</v>
@@ -17664,7 +17673,7 @@
         <v>634</v>
       </c>
       <c r="E77" s="60" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="F77" s="25" t="s">
         <v>460</v>
@@ -17682,7 +17691,7 @@
         <v>635</v>
       </c>
       <c r="E78" s="60" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="F78" s="25" t="s">
         <v>461</v>
@@ -17695,11 +17704,11 @@
       <c r="B79" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="C79" s="112" t="s">
+      <c r="C79" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D79" s="113"/>
-      <c r="E79" s="114"/>
+      <c r="D79" s="89"/>
+      <c r="E79" s="90"/>
       <c r="F79" s="25" t="s">
         <v>462</v>
       </c>
@@ -17711,9 +17720,9 @@
       <c r="B80" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C80" s="121"/>
-      <c r="D80" s="122"/>
-      <c r="E80" s="123"/>
+      <c r="C80" s="91"/>
+      <c r="D80" s="92"/>
+      <c r="E80" s="93"/>
       <c r="F80" s="25" t="s">
         <v>463</v>
       </c>
@@ -17725,9 +17734,9 @@
       <c r="B81" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C81" s="121"/>
-      <c r="D81" s="122"/>
-      <c r="E81" s="123"/>
+      <c r="C81" s="91"/>
+      <c r="D81" s="92"/>
+      <c r="E81" s="93"/>
       <c r="F81" s="26" t="s">
         <v>464</v>
       </c>
@@ -17739,9 +17748,9 @@
       <c r="B82" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C82" s="121"/>
-      <c r="D82" s="122"/>
-      <c r="E82" s="123"/>
+      <c r="C82" s="91"/>
+      <c r="D82" s="92"/>
+      <c r="E82" s="93"/>
       <c r="F82" s="26" t="s">
         <v>465</v>
       </c>
@@ -17753,9 +17762,9 @@
       <c r="B83" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="C83" s="121"/>
-      <c r="D83" s="122"/>
-      <c r="E83" s="123"/>
+      <c r="C83" s="91"/>
+      <c r="D83" s="92"/>
+      <c r="E83" s="93"/>
       <c r="F83" s="26" t="s">
         <v>466</v>
       </c>
@@ -17767,9 +17776,9 @@
       <c r="B84" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="C84" s="121"/>
-      <c r="D84" s="122"/>
-      <c r="E84" s="123"/>
+      <c r="C84" s="91"/>
+      <c r="D84" s="92"/>
+      <c r="E84" s="93"/>
       <c r="F84" s="26" t="s">
         <v>467</v>
       </c>
@@ -17781,9 +17790,9 @@
       <c r="B85" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="C85" s="115"/>
-      <c r="D85" s="116"/>
-      <c r="E85" s="117"/>
+      <c r="C85" s="94"/>
+      <c r="D85" s="95"/>
+      <c r="E85" s="96"/>
       <c r="F85" s="26" t="s">
         <v>468</v>
       </c>
@@ -17800,7 +17809,7 @@
         <v>636</v>
       </c>
       <c r="E86" s="60" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F86" s="26" t="s">
         <v>469</v>
@@ -17818,7 +17827,7 @@
         <v>643</v>
       </c>
       <c r="E87" s="60" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F87" s="26" t="s">
         <v>470</v>
@@ -17836,7 +17845,7 @@
         <v>637</v>
       </c>
       <c r="E88" s="60" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F88" s="26" t="s">
         <v>471</v>
@@ -17854,7 +17863,7 @@
         <v>638</v>
       </c>
       <c r="E89" s="60" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F89" s="26" t="s">
         <v>472</v>
@@ -17872,7 +17881,7 @@
         <v>644</v>
       </c>
       <c r="E90" s="60" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="F90" s="26" t="s">
         <v>473</v>
@@ -17890,7 +17899,7 @@
         <v>645</v>
       </c>
       <c r="E91" s="60" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F91" s="26" t="s">
         <v>474</v>
@@ -17908,7 +17917,7 @@
         <v>646</v>
       </c>
       <c r="E92" s="60" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F92" s="26" t="s">
         <v>475</v>
@@ -17926,7 +17935,7 @@
         <v>647</v>
       </c>
       <c r="E93" s="60" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F93" s="26" t="s">
         <v>476</v>
@@ -17944,7 +17953,7 @@
         <v>639</v>
       </c>
       <c r="E94" s="60" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F94" s="26" t="s">
         <v>477</v>
@@ -17962,7 +17971,7 @@
         <v>640</v>
       </c>
       <c r="E95" s="60" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="F95" s="26" t="s">
         <v>478</v>
@@ -17980,7 +17989,7 @@
         <v>641</v>
       </c>
       <c r="E96" s="60" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F96" s="26" t="s">
         <v>479</v>
@@ -17998,7 +18007,7 @@
         <v>642</v>
       </c>
       <c r="E97" s="60" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F97" s="26" t="s">
         <v>480</v>
@@ -18008,63 +18017,63 @@
       <c r="A98" s="27">
         <v>96</v>
       </c>
-      <c r="B98" s="100" t="s">
+      <c r="B98" s="97" t="s">
         <v>433</v>
       </c>
-      <c r="C98" s="101"/>
-      <c r="D98" s="101"/>
-      <c r="E98" s="101"/>
-      <c r="F98" s="102"/>
+      <c r="C98" s="98"/>
+      <c r="D98" s="98"/>
+      <c r="E98" s="98"/>
+      <c r="F98" s="99"/>
     </row>
     <row r="99" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="27">
         <v>97</v>
       </c>
-      <c r="B99" s="103"/>
-      <c r="C99" s="104"/>
-      <c r="D99" s="104"/>
-      <c r="E99" s="104"/>
-      <c r="F99" s="105"/>
+      <c r="B99" s="100"/>
+      <c r="C99" s="101"/>
+      <c r="D99" s="101"/>
+      <c r="E99" s="101"/>
+      <c r="F99" s="102"/>
     </row>
     <row r="100" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="27">
         <v>98</v>
       </c>
-      <c r="B100" s="103"/>
-      <c r="C100" s="104"/>
-      <c r="D100" s="104"/>
-      <c r="E100" s="104"/>
-      <c r="F100" s="105"/>
+      <c r="B100" s="100"/>
+      <c r="C100" s="101"/>
+      <c r="D100" s="101"/>
+      <c r="E100" s="101"/>
+      <c r="F100" s="102"/>
     </row>
     <row r="101" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="27">
         <v>99</v>
       </c>
-      <c r="B101" s="103"/>
-      <c r="C101" s="104"/>
-      <c r="D101" s="104"/>
-      <c r="E101" s="104"/>
-      <c r="F101" s="105"/>
+      <c r="B101" s="100"/>
+      <c r="C101" s="101"/>
+      <c r="D101" s="101"/>
+      <c r="E101" s="101"/>
+      <c r="F101" s="102"/>
     </row>
     <row r="102" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="27">
         <v>100</v>
       </c>
-      <c r="B102" s="103"/>
-      <c r="C102" s="104"/>
-      <c r="D102" s="104"/>
-      <c r="E102" s="104"/>
-      <c r="F102" s="105"/>
+      <c r="B102" s="100"/>
+      <c r="C102" s="101"/>
+      <c r="D102" s="101"/>
+      <c r="E102" s="101"/>
+      <c r="F102" s="102"/>
     </row>
     <row r="103" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="27">
         <v>101</v>
       </c>
-      <c r="B103" s="106"/>
-      <c r="C103" s="107"/>
-      <c r="D103" s="107"/>
-      <c r="E103" s="107"/>
-      <c r="F103" s="108"/>
+      <c r="B103" s="103"/>
+      <c r="C103" s="104"/>
+      <c r="D103" s="104"/>
+      <c r="E103" s="104"/>
+      <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="24">
@@ -18073,11 +18082,11 @@
       <c r="B104" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="C104" s="112" t="s">
+      <c r="C104" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D104" s="113"/>
-      <c r="E104" s="114"/>
+      <c r="D104" s="89"/>
+      <c r="E104" s="90"/>
       <c r="F104" s="26" t="s">
         <v>481</v>
       </c>
@@ -18089,9 +18098,9 @@
       <c r="B105" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="C105" s="121"/>
-      <c r="D105" s="122"/>
-      <c r="E105" s="123"/>
+      <c r="C105" s="91"/>
+      <c r="D105" s="92"/>
+      <c r="E105" s="93"/>
       <c r="F105" s="26" t="s">
         <v>482</v>
       </c>
@@ -18103,9 +18112,9 @@
       <c r="B106" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="C106" s="115"/>
-      <c r="D106" s="116"/>
-      <c r="E106" s="117"/>
+      <c r="C106" s="94"/>
+      <c r="D106" s="95"/>
+      <c r="E106" s="96"/>
       <c r="F106" s="26" t="s">
         <v>483</v>
       </c>
@@ -18122,7 +18131,7 @@
         <v>648</v>
       </c>
       <c r="E107" s="60" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F107" s="26" t="s">
         <v>484</v>
@@ -18156,7 +18165,7 @@
         <v>650</v>
       </c>
       <c r="E109" s="60" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F109" s="25" t="s">
         <v>486</v>
@@ -18174,7 +18183,7 @@
         <v>651</v>
       </c>
       <c r="E110" s="60" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F110" s="25" t="s">
         <v>487</v>
@@ -18192,7 +18201,7 @@
         <v>652</v>
       </c>
       <c r="E111" s="60" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F111" s="25" t="s">
         <v>488</v>
@@ -18210,7 +18219,7 @@
         <v>653</v>
       </c>
       <c r="E112" s="60" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F112" s="25" t="s">
         <v>489</v>
@@ -18223,11 +18232,11 @@
       <c r="B113" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="C113" s="112" t="s">
+      <c r="C113" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D113" s="113"/>
-      <c r="E113" s="114"/>
+      <c r="D113" s="89"/>
+      <c r="E113" s="90"/>
       <c r="F113" s="25" t="s">
         <v>490</v>
       </c>
@@ -18239,9 +18248,9 @@
       <c r="B114" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="C114" s="115"/>
-      <c r="D114" s="116"/>
-      <c r="E114" s="117"/>
+      <c r="C114" s="94"/>
+      <c r="D114" s="95"/>
+      <c r="E114" s="96"/>
       <c r="F114" s="25" t="s">
         <v>491</v>
       </c>
@@ -18258,7 +18267,7 @@
         <v>654</v>
       </c>
       <c r="E115" s="60" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F115" s="25" t="s">
         <v>492</v>
@@ -18276,7 +18285,7 @@
         <v>655</v>
       </c>
       <c r="E116" s="60" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F116" s="25" t="s">
         <v>493</v>
@@ -18294,7 +18303,7 @@
         <v>656</v>
       </c>
       <c r="E117" s="60" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F117" s="25" t="s">
         <v>494</v>
@@ -18312,7 +18321,7 @@
         <v>657</v>
       </c>
       <c r="E118" s="60" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F118" s="25" t="s">
         <v>495</v>
@@ -18330,7 +18339,7 @@
         <v>658</v>
       </c>
       <c r="E119" s="60" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F119" s="25" t="s">
         <v>496</v>
@@ -18348,7 +18357,7 @@
         <v>659</v>
       </c>
       <c r="E120" s="60" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="F120" s="25" t="s">
         <v>497</v>
@@ -18366,7 +18375,7 @@
         <v>660</v>
       </c>
       <c r="E121" s="60" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F121" s="25" t="s">
         <v>498</v>
@@ -18384,7 +18393,7 @@
         <v>661</v>
       </c>
       <c r="E122" s="60" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F122" s="25" t="s">
         <v>420</v>
@@ -18402,7 +18411,7 @@
         <v>663</v>
       </c>
       <c r="E123" s="60" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F123" s="25" t="s">
         <v>420</v>
@@ -18420,7 +18429,7 @@
         <v>662</v>
       </c>
       <c r="E124" s="60" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="F124" s="25" t="s">
         <v>420</v>
@@ -18438,7 +18447,7 @@
         <v>664</v>
       </c>
       <c r="E125" s="60" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F125" s="25" t="s">
         <v>420</v>
@@ -18456,7 +18465,7 @@
         <v>665</v>
       </c>
       <c r="E126" s="60" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F126" s="25" t="s">
         <v>499</v>
@@ -18474,7 +18483,7 @@
         <v>666</v>
       </c>
       <c r="E127" s="60" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="F127" s="25" t="s">
         <v>500</v>
@@ -18492,7 +18501,7 @@
         <v>667</v>
       </c>
       <c r="E128" s="60" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F128" s="25" t="s">
         <v>501</v>
@@ -18505,11 +18514,11 @@
       <c r="B129" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="C129" s="118" t="s">
+      <c r="C129" s="85" t="s">
         <v>583</v>
       </c>
-      <c r="D129" s="119"/>
-      <c r="E129" s="120"/>
+      <c r="D129" s="86"/>
+      <c r="E129" s="87"/>
       <c r="F129" s="25" t="s">
         <v>502</v>
       </c>
@@ -18518,63 +18527,63 @@
       <c r="A130" s="27">
         <v>128</v>
       </c>
-      <c r="B130" s="100" t="s">
+      <c r="B130" s="97" t="s">
         <v>433</v>
       </c>
-      <c r="C130" s="101"/>
-      <c r="D130" s="101"/>
-      <c r="E130" s="101"/>
-      <c r="F130" s="102"/>
+      <c r="C130" s="98"/>
+      <c r="D130" s="98"/>
+      <c r="E130" s="98"/>
+      <c r="F130" s="99"/>
     </row>
     <row r="131" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="27">
         <v>129</v>
       </c>
-      <c r="B131" s="103"/>
-      <c r="C131" s="104"/>
-      <c r="D131" s="104"/>
-      <c r="E131" s="104"/>
-      <c r="F131" s="105"/>
+      <c r="B131" s="100"/>
+      <c r="C131" s="101"/>
+      <c r="D131" s="101"/>
+      <c r="E131" s="101"/>
+      <c r="F131" s="102"/>
     </row>
     <row r="132" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="27">
         <v>130</v>
       </c>
-      <c r="B132" s="103"/>
-      <c r="C132" s="104"/>
-      <c r="D132" s="104"/>
-      <c r="E132" s="104"/>
-      <c r="F132" s="105"/>
+      <c r="B132" s="100"/>
+      <c r="C132" s="101"/>
+      <c r="D132" s="101"/>
+      <c r="E132" s="101"/>
+      <c r="F132" s="102"/>
     </row>
     <row r="133" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="27">
         <v>131</v>
       </c>
-      <c r="B133" s="103"/>
-      <c r="C133" s="104"/>
-      <c r="D133" s="104"/>
-      <c r="E133" s="104"/>
-      <c r="F133" s="105"/>
+      <c r="B133" s="100"/>
+      <c r="C133" s="101"/>
+      <c r="D133" s="101"/>
+      <c r="E133" s="101"/>
+      <c r="F133" s="102"/>
     </row>
     <row r="134" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="27">
         <v>132</v>
       </c>
-      <c r="B134" s="103"/>
-      <c r="C134" s="104"/>
-      <c r="D134" s="104"/>
-      <c r="E134" s="104"/>
-      <c r="F134" s="105"/>
+      <c r="B134" s="100"/>
+      <c r="C134" s="101"/>
+      <c r="D134" s="101"/>
+      <c r="E134" s="101"/>
+      <c r="F134" s="102"/>
     </row>
     <row r="135" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="27">
         <v>133</v>
       </c>
-      <c r="B135" s="106"/>
-      <c r="C135" s="107"/>
-      <c r="D135" s="107"/>
-      <c r="E135" s="107"/>
-      <c r="F135" s="108"/>
+      <c r="B135" s="103"/>
+      <c r="C135" s="104"/>
+      <c r="D135" s="104"/>
+      <c r="E135" s="104"/>
+      <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="24">
@@ -18588,7 +18597,7 @@
         <v>668</v>
       </c>
       <c r="E136" s="60" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F136" s="25" t="s">
         <v>503</v>
@@ -18606,7 +18615,7 @@
         <v>674</v>
       </c>
       <c r="E137" s="60" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F137" s="25" t="s">
         <v>504</v>
@@ -18624,7 +18633,7 @@
         <v>669</v>
       </c>
       <c r="E138" s="60" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F138" s="25" t="s">
         <v>505</v>
@@ -18642,7 +18651,7 @@
         <v>675</v>
       </c>
       <c r="E139" s="60" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F139" s="25" t="s">
         <v>506</v>
@@ -18660,7 +18669,7 @@
         <v>670</v>
       </c>
       <c r="E140" s="60" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F140" s="25" t="s">
         <v>507</v>
@@ -18678,7 +18687,7 @@
         <v>676</v>
       </c>
       <c r="E141" s="60" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F141" s="25" t="s">
         <v>508</v>
@@ -18696,7 +18705,7 @@
         <v>671</v>
       </c>
       <c r="E142" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F142" s="25" t="s">
         <v>509</v>
@@ -18714,7 +18723,7 @@
         <v>677</v>
       </c>
       <c r="E143" s="60" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F143" s="25" t="s">
         <v>510</v>
@@ -18732,7 +18741,7 @@
         <v>672</v>
       </c>
       <c r="E144" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="F144" s="25" t="s">
         <v>511</v>
@@ -18750,7 +18759,7 @@
         <v>678</v>
       </c>
       <c r="E145" s="60" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="F145" s="25" t="s">
         <v>512</v>
@@ -18768,7 +18777,7 @@
         <v>673</v>
       </c>
       <c r="E146" s="60" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F146" s="25" t="s">
         <v>513</v>
@@ -18786,7 +18795,7 @@
         <v>679</v>
       </c>
       <c r="E147" s="60" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F147" s="25" t="s">
         <v>514</v>
@@ -18804,7 +18813,7 @@
         <v>680</v>
       </c>
       <c r="E148" s="60" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F148" s="25" t="s">
         <v>515</v>
@@ -18822,7 +18831,7 @@
         <v>681</v>
       </c>
       <c r="E149" s="60" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="F149" s="25" t="s">
         <v>516</v>
@@ -18840,7 +18849,7 @@
         <v>682</v>
       </c>
       <c r="E150" s="60" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F150" s="25" t="s">
         <v>517</v>
@@ -18860,7 +18869,7 @@
         <v>683</v>
       </c>
       <c r="E151" s="60" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F151" s="25" t="s">
         <v>518</v>
@@ -18878,7 +18887,7 @@
         <v>684</v>
       </c>
       <c r="E152" s="60" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="F152" s="25" t="s">
         <v>393</v>
@@ -18896,7 +18905,7 @@
         <v>685</v>
       </c>
       <c r="E153" s="60" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F153" s="25" t="s">
         <v>519</v>
@@ -18914,7 +18923,7 @@
         <v>686</v>
       </c>
       <c r="E154" s="60" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="F154" s="25" t="s">
         <v>520</v>
@@ -18927,11 +18936,11 @@
       <c r="B155" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="C155" s="112" t="s">
+      <c r="C155" s="88" t="s">
         <v>583</v>
       </c>
-      <c r="D155" s="113"/>
-      <c r="E155" s="114"/>
+      <c r="D155" s="89"/>
+      <c r="E155" s="90"/>
       <c r="F155" s="25" t="s">
         <v>521</v>
       </c>
@@ -18943,9 +18952,9 @@
       <c r="B156" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="C156" s="115"/>
-      <c r="D156" s="116"/>
-      <c r="E156" s="117"/>
+      <c r="C156" s="94"/>
+      <c r="D156" s="95"/>
+      <c r="E156" s="96"/>
       <c r="F156" s="25" t="s">
         <v>522</v>
       </c>
@@ -18954,13 +18963,13 @@
       <c r="A157" s="27">
         <v>155</v>
       </c>
-      <c r="B157" s="109" t="s">
+      <c r="B157" s="106" t="s">
         <v>433</v>
       </c>
-      <c r="C157" s="110"/>
-      <c r="D157" s="110"/>
-      <c r="E157" s="110"/>
-      <c r="F157" s="111"/>
+      <c r="C157" s="107"/>
+      <c r="D157" s="107"/>
+      <c r="E157" s="107"/>
+      <c r="F157" s="108"/>
     </row>
     <row r="158" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="24">
@@ -18969,11 +18978,11 @@
       <c r="B158" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="C158" s="118" t="s">
+      <c r="C158" s="85" t="s">
         <v>583</v>
       </c>
-      <c r="D158" s="119"/>
-      <c r="E158" s="120"/>
+      <c r="D158" s="86"/>
+      <c r="E158" s="87"/>
       <c r="F158" s="25" t="s">
         <v>523</v>
       </c>
@@ -18990,7 +18999,7 @@
         <v>687</v>
       </c>
       <c r="E159" s="60" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F159" s="25" t="s">
         <v>524</v>
@@ -19008,7 +19017,7 @@
         <v>688</v>
       </c>
       <c r="E160" s="60" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F160" s="25" t="s">
         <v>525</v>
@@ -19026,7 +19035,7 @@
         <v>689</v>
       </c>
       <c r="E161" s="60" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F161" s="25" t="s">
         <v>526</v>
@@ -19044,7 +19053,7 @@
         <v>690</v>
       </c>
       <c r="E162" s="60" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="F162" s="25" t="s">
         <v>527</v>
@@ -19062,7 +19071,7 @@
         <v>691</v>
       </c>
       <c r="E163" s="60" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="F163" s="25" t="s">
         <v>528</v>
@@ -19080,7 +19089,7 @@
         <v>692</v>
       </c>
       <c r="E164" s="60" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="F164" s="25" t="s">
         <v>529</v>
@@ -19098,7 +19107,7 @@
         <v>693</v>
       </c>
       <c r="E165" s="60" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F165" s="25" t="s">
         <v>530</v>
@@ -19108,123 +19117,123 @@
       <c r="A166" s="27">
         <v>164</v>
       </c>
-      <c r="B166" s="100" t="s">
+      <c r="B166" s="97" t="s">
         <v>433</v>
       </c>
-      <c r="C166" s="101"/>
-      <c r="D166" s="101"/>
-      <c r="E166" s="101"/>
-      <c r="F166" s="102"/>
+      <c r="C166" s="98"/>
+      <c r="D166" s="98"/>
+      <c r="E166" s="98"/>
+      <c r="F166" s="99"/>
     </row>
     <row r="167" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A167" s="27">
         <v>165</v>
       </c>
-      <c r="B167" s="103"/>
-      <c r="C167" s="104"/>
-      <c r="D167" s="104"/>
-      <c r="E167" s="104"/>
-      <c r="F167" s="105"/>
+      <c r="B167" s="100"/>
+      <c r="C167" s="101"/>
+      <c r="D167" s="101"/>
+      <c r="E167" s="101"/>
+      <c r="F167" s="102"/>
     </row>
     <row r="168" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A168" s="27">
         <v>166</v>
       </c>
-      <c r="B168" s="103"/>
-      <c r="C168" s="104"/>
-      <c r="D168" s="104"/>
-      <c r="E168" s="104"/>
-      <c r="F168" s="105"/>
+      <c r="B168" s="100"/>
+      <c r="C168" s="101"/>
+      <c r="D168" s="101"/>
+      <c r="E168" s="101"/>
+      <c r="F168" s="102"/>
     </row>
     <row r="169" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A169" s="27">
         <v>167</v>
       </c>
-      <c r="B169" s="103"/>
-      <c r="C169" s="104"/>
-      <c r="D169" s="104"/>
-      <c r="E169" s="104"/>
-      <c r="F169" s="105"/>
+      <c r="B169" s="100"/>
+      <c r="C169" s="101"/>
+      <c r="D169" s="101"/>
+      <c r="E169" s="101"/>
+      <c r="F169" s="102"/>
     </row>
     <row r="170" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A170" s="27">
         <v>168</v>
       </c>
-      <c r="B170" s="103"/>
-      <c r="C170" s="104"/>
-      <c r="D170" s="104"/>
-      <c r="E170" s="104"/>
-      <c r="F170" s="105"/>
+      <c r="B170" s="100"/>
+      <c r="C170" s="101"/>
+      <c r="D170" s="101"/>
+      <c r="E170" s="101"/>
+      <c r="F170" s="102"/>
     </row>
     <row r="171" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A171" s="27">
         <v>169</v>
       </c>
-      <c r="B171" s="103"/>
-      <c r="C171" s="104"/>
-      <c r="D171" s="104"/>
-      <c r="E171" s="104"/>
-      <c r="F171" s="105"/>
+      <c r="B171" s="100"/>
+      <c r="C171" s="101"/>
+      <c r="D171" s="101"/>
+      <c r="E171" s="101"/>
+      <c r="F171" s="102"/>
     </row>
     <row r="172" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A172" s="27">
         <v>170</v>
       </c>
-      <c r="B172" s="103"/>
-      <c r="C172" s="104"/>
-      <c r="D172" s="104"/>
-      <c r="E172" s="104"/>
-      <c r="F172" s="105"/>
+      <c r="B172" s="100"/>
+      <c r="C172" s="101"/>
+      <c r="D172" s="101"/>
+      <c r="E172" s="101"/>
+      <c r="F172" s="102"/>
     </row>
     <row r="173" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A173" s="27">
         <v>171</v>
       </c>
-      <c r="B173" s="103"/>
-      <c r="C173" s="104"/>
-      <c r="D173" s="104"/>
-      <c r="E173" s="104"/>
-      <c r="F173" s="105"/>
+      <c r="B173" s="100"/>
+      <c r="C173" s="101"/>
+      <c r="D173" s="101"/>
+      <c r="E173" s="101"/>
+      <c r="F173" s="102"/>
     </row>
     <row r="174" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A174" s="27">
         <v>172</v>
       </c>
-      <c r="B174" s="103"/>
-      <c r="C174" s="104"/>
-      <c r="D174" s="104"/>
-      <c r="E174" s="104"/>
-      <c r="F174" s="105"/>
+      <c r="B174" s="100"/>
+      <c r="C174" s="101"/>
+      <c r="D174" s="101"/>
+      <c r="E174" s="101"/>
+      <c r="F174" s="102"/>
     </row>
     <row r="175" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A175" s="27">
         <v>173</v>
       </c>
-      <c r="B175" s="103"/>
-      <c r="C175" s="104"/>
-      <c r="D175" s="104"/>
-      <c r="E175" s="104"/>
-      <c r="F175" s="105"/>
+      <c r="B175" s="100"/>
+      <c r="C175" s="101"/>
+      <c r="D175" s="101"/>
+      <c r="E175" s="101"/>
+      <c r="F175" s="102"/>
     </row>
     <row r="176" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A176" s="27">
         <v>174</v>
       </c>
-      <c r="B176" s="103"/>
-      <c r="C176" s="104"/>
-      <c r="D176" s="104"/>
-      <c r="E176" s="104"/>
-      <c r="F176" s="105"/>
+      <c r="B176" s="100"/>
+      <c r="C176" s="101"/>
+      <c r="D176" s="101"/>
+      <c r="E176" s="101"/>
+      <c r="F176" s="102"/>
     </row>
     <row r="177" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" s="27">
         <v>175</v>
       </c>
-      <c r="B177" s="106"/>
-      <c r="C177" s="107"/>
-      <c r="D177" s="107"/>
-      <c r="E177" s="107"/>
-      <c r="F177" s="108"/>
+      <c r="B177" s="103"/>
+      <c r="C177" s="104"/>
+      <c r="D177" s="104"/>
+      <c r="E177" s="104"/>
+      <c r="F177" s="105"/>
     </row>
     <row r="178" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="24">
@@ -19238,7 +19247,7 @@
         <v>694</v>
       </c>
       <c r="E178" s="60" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="F178" s="25" t="s">
         <v>531</v>
@@ -19256,7 +19265,7 @@
         <v>700</v>
       </c>
       <c r="E179" s="60" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="F179" s="25" t="s">
         <v>532</v>
@@ -19274,7 +19283,7 @@
         <v>708</v>
       </c>
       <c r="E180" s="60" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="F180" s="25" t="s">
         <v>533</v>
@@ -19292,7 +19301,7 @@
         <v>709</v>
       </c>
       <c r="E181" s="60" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="F181" s="25" t="s">
         <v>534</v>
@@ -19310,7 +19319,7 @@
         <v>695</v>
       </c>
       <c r="E182" s="60" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="F182" s="25" t="s">
         <v>535</v>
@@ -19328,7 +19337,7 @@
         <v>711</v>
       </c>
       <c r="E183" s="60" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="F183" s="25" t="s">
         <v>536</v>
@@ -19346,7 +19355,7 @@
         <v>712</v>
       </c>
       <c r="E184" s="60" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="F184" s="25" t="s">
         <v>537</v>
@@ -19364,7 +19373,7 @@
         <v>696</v>
       </c>
       <c r="E185" s="60" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F185" s="25" t="s">
         <v>538</v>
@@ -19382,7 +19391,7 @@
         <v>697</v>
       </c>
       <c r="E186" s="60" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="F186" s="25" t="s">
         <v>539</v>
@@ -19400,7 +19409,7 @@
         <v>698</v>
       </c>
       <c r="E187" s="60" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="F187" s="25" t="s">
         <v>540</v>
@@ -19418,7 +19427,7 @@
         <v>699</v>
       </c>
       <c r="E188" s="60" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F188" s="25" t="s">
         <v>541</v>
@@ -19436,7 +19445,7 @@
         <v>701</v>
       </c>
       <c r="E189" s="60" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="F189" s="25" t="s">
         <v>542</v>
@@ -19454,7 +19463,7 @@
         <v>702</v>
       </c>
       <c r="E190" s="60" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="F190" s="25" t="s">
         <v>543</v>
@@ -19472,7 +19481,7 @@
         <v>703</v>
       </c>
       <c r="E191" s="60" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="F191" s="25" t="s">
         <v>544</v>
@@ -19490,7 +19499,7 @@
         <v>704</v>
       </c>
       <c r="E192" s="60" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="F192" s="25" t="s">
         <v>545</v>
@@ -19508,7 +19517,7 @@
         <v>705</v>
       </c>
       <c r="E193" s="60" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="F193" s="25" t="s">
         <v>546</v>
@@ -19526,7 +19535,7 @@
         <v>706</v>
       </c>
       <c r="E194" s="60" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="F194" s="25" t="s">
         <v>547</v>
@@ -19544,7 +19553,7 @@
         <v>707</v>
       </c>
       <c r="E195" s="60" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="F195" s="25" t="s">
         <v>548</v>
@@ -19562,7 +19571,7 @@
         <v>710</v>
       </c>
       <c r="E196" s="60" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F196" s="25" t="s">
         <v>549</v>
@@ -19580,7 +19589,7 @@
         <v>713</v>
       </c>
       <c r="E197" s="60" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="F197" s="25" t="s">
         <v>550</v>
@@ -19598,7 +19607,7 @@
         <v>714</v>
       </c>
       <c r="E198" s="60" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="F198" s="25" t="s">
         <v>551</v>
@@ -19608,13 +19617,13 @@
       <c r="A199" s="27">
         <v>197</v>
       </c>
-      <c r="B199" s="109" t="s">
+      <c r="B199" s="106" t="s">
         <v>569</v>
       </c>
-      <c r="C199" s="110"/>
-      <c r="D199" s="110"/>
-      <c r="E199" s="110"/>
-      <c r="F199" s="111"/>
+      <c r="C199" s="107"/>
+      <c r="D199" s="107"/>
+      <c r="E199" s="107"/>
+      <c r="F199" s="108"/>
     </row>
     <row r="200" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A200" s="24">
@@ -19628,7 +19637,7 @@
         <v>715</v>
       </c>
       <c r="E200" s="60" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="F200" s="25" t="s">
         <v>420</v>
@@ -19638,103 +19647,103 @@
       <c r="A201" s="27">
         <v>199</v>
       </c>
-      <c r="B201" s="100" t="s">
+      <c r="B201" s="97" t="s">
         <v>568</v>
       </c>
-      <c r="C201" s="101"/>
-      <c r="D201" s="101"/>
-      <c r="E201" s="101"/>
-      <c r="F201" s="102"/>
+      <c r="C201" s="98"/>
+      <c r="D201" s="98"/>
+      <c r="E201" s="98"/>
+      <c r="F201" s="99"/>
     </row>
     <row r="202" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A202" s="27">
         <v>200</v>
       </c>
-      <c r="B202" s="103"/>
-      <c r="C202" s="104"/>
-      <c r="D202" s="104"/>
-      <c r="E202" s="104"/>
-      <c r="F202" s="105"/>
+      <c r="B202" s="100"/>
+      <c r="C202" s="101"/>
+      <c r="D202" s="101"/>
+      <c r="E202" s="101"/>
+      <c r="F202" s="102"/>
     </row>
     <row r="203" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A203" s="27">
         <v>201</v>
       </c>
-      <c r="B203" s="103"/>
-      <c r="C203" s="104"/>
-      <c r="D203" s="104"/>
-      <c r="E203" s="104"/>
-      <c r="F203" s="105"/>
+      <c r="B203" s="100"/>
+      <c r="C203" s="101"/>
+      <c r="D203" s="101"/>
+      <c r="E203" s="101"/>
+      <c r="F203" s="102"/>
     </row>
     <row r="204" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A204" s="27">
         <v>202</v>
       </c>
-      <c r="B204" s="103"/>
-      <c r="C204" s="104"/>
-      <c r="D204" s="104"/>
-      <c r="E204" s="104"/>
-      <c r="F204" s="105"/>
+      <c r="B204" s="100"/>
+      <c r="C204" s="101"/>
+      <c r="D204" s="101"/>
+      <c r="E204" s="101"/>
+      <c r="F204" s="102"/>
     </row>
     <row r="205" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A205" s="27">
         <v>203</v>
       </c>
-      <c r="B205" s="103"/>
-      <c r="C205" s="104"/>
-      <c r="D205" s="104"/>
-      <c r="E205" s="104"/>
-      <c r="F205" s="105"/>
+      <c r="B205" s="100"/>
+      <c r="C205" s="101"/>
+      <c r="D205" s="101"/>
+      <c r="E205" s="101"/>
+      <c r="F205" s="102"/>
     </row>
     <row r="206" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A206" s="27">
         <v>204</v>
       </c>
-      <c r="B206" s="103"/>
-      <c r="C206" s="104"/>
-      <c r="D206" s="104"/>
-      <c r="E206" s="104"/>
-      <c r="F206" s="105"/>
+      <c r="B206" s="100"/>
+      <c r="C206" s="101"/>
+      <c r="D206" s="101"/>
+      <c r="E206" s="101"/>
+      <c r="F206" s="102"/>
     </row>
     <row r="207" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A207" s="27">
         <v>205</v>
       </c>
-      <c r="B207" s="103"/>
-      <c r="C207" s="104"/>
-      <c r="D207" s="104"/>
-      <c r="E207" s="104"/>
-      <c r="F207" s="105"/>
+      <c r="B207" s="100"/>
+      <c r="C207" s="101"/>
+      <c r="D207" s="101"/>
+      <c r="E207" s="101"/>
+      <c r="F207" s="102"/>
     </row>
     <row r="208" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A208" s="27">
         <v>206</v>
       </c>
-      <c r="B208" s="103"/>
-      <c r="C208" s="104"/>
-      <c r="D208" s="104"/>
-      <c r="E208" s="104"/>
-      <c r="F208" s="105"/>
+      <c r="B208" s="100"/>
+      <c r="C208" s="101"/>
+      <c r="D208" s="101"/>
+      <c r="E208" s="101"/>
+      <c r="F208" s="102"/>
     </row>
     <row r="209" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A209" s="27">
         <v>207</v>
       </c>
-      <c r="B209" s="103"/>
-      <c r="C209" s="104"/>
-      <c r="D209" s="104"/>
-      <c r="E209" s="104"/>
-      <c r="F209" s="105"/>
+      <c r="B209" s="100"/>
+      <c r="C209" s="101"/>
+      <c r="D209" s="101"/>
+      <c r="E209" s="101"/>
+      <c r="F209" s="102"/>
     </row>
     <row r="210" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A210" s="27">
         <v>208</v>
       </c>
-      <c r="B210" s="106"/>
-      <c r="C210" s="107"/>
-      <c r="D210" s="107"/>
-      <c r="E210" s="107"/>
-      <c r="F210" s="108"/>
+      <c r="B210" s="103"/>
+      <c r="C210" s="104"/>
+      <c r="D210" s="104"/>
+      <c r="E210" s="104"/>
+      <c r="F210" s="105"/>
     </row>
     <row r="211" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A211" s="24">
@@ -19750,7 +19759,7 @@
         <v>716</v>
       </c>
       <c r="E211" s="60" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="F211" s="25" t="s">
         <v>553</v>
@@ -19784,7 +19793,7 @@
         <v>718</v>
       </c>
       <c r="E213" s="60" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F213" s="25" t="s">
         <v>555</v>
@@ -19794,83 +19803,83 @@
       <c r="A214" s="27">
         <v>212</v>
       </c>
-      <c r="B214" s="100" t="s">
+      <c r="B214" s="97" t="s">
         <v>552</v>
       </c>
-      <c r="C214" s="101"/>
-      <c r="D214" s="101"/>
-      <c r="E214" s="101"/>
-      <c r="F214" s="102"/>
+      <c r="C214" s="98"/>
+      <c r="D214" s="98"/>
+      <c r="E214" s="98"/>
+      <c r="F214" s="99"/>
     </row>
     <row r="215" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A215" s="27">
         <v>213</v>
       </c>
-      <c r="B215" s="103"/>
-      <c r="C215" s="104"/>
-      <c r="D215" s="104"/>
-      <c r="E215" s="104"/>
-      <c r="F215" s="105"/>
+      <c r="B215" s="100"/>
+      <c r="C215" s="101"/>
+      <c r="D215" s="101"/>
+      <c r="E215" s="101"/>
+      <c r="F215" s="102"/>
     </row>
     <row r="216" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A216" s="27">
         <v>214</v>
       </c>
-      <c r="B216" s="103"/>
-      <c r="C216" s="104"/>
-      <c r="D216" s="104"/>
-      <c r="E216" s="104"/>
-      <c r="F216" s="105"/>
+      <c r="B216" s="100"/>
+      <c r="C216" s="101"/>
+      <c r="D216" s="101"/>
+      <c r="E216" s="101"/>
+      <c r="F216" s="102"/>
     </row>
     <row r="217" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A217" s="27">
         <v>215</v>
       </c>
-      <c r="B217" s="103"/>
-      <c r="C217" s="104"/>
-      <c r="D217" s="104"/>
-      <c r="E217" s="104"/>
-      <c r="F217" s="105"/>
+      <c r="B217" s="100"/>
+      <c r="C217" s="101"/>
+      <c r="D217" s="101"/>
+      <c r="E217" s="101"/>
+      <c r="F217" s="102"/>
     </row>
     <row r="218" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A218" s="27">
         <v>216</v>
       </c>
-      <c r="B218" s="103"/>
-      <c r="C218" s="104"/>
-      <c r="D218" s="104"/>
-      <c r="E218" s="104"/>
-      <c r="F218" s="105"/>
+      <c r="B218" s="100"/>
+      <c r="C218" s="101"/>
+      <c r="D218" s="101"/>
+      <c r="E218" s="101"/>
+      <c r="F218" s="102"/>
     </row>
     <row r="219" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A219" s="27">
         <v>217</v>
       </c>
-      <c r="B219" s="103"/>
-      <c r="C219" s="104"/>
-      <c r="D219" s="104"/>
-      <c r="E219" s="104"/>
-      <c r="F219" s="105"/>
+      <c r="B219" s="100"/>
+      <c r="C219" s="101"/>
+      <c r="D219" s="101"/>
+      <c r="E219" s="101"/>
+      <c r="F219" s="102"/>
     </row>
     <row r="220" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A220" s="27">
         <v>218</v>
       </c>
-      <c r="B220" s="103"/>
-      <c r="C220" s="104"/>
-      <c r="D220" s="104"/>
-      <c r="E220" s="104"/>
-      <c r="F220" s="105"/>
+      <c r="B220" s="100"/>
+      <c r="C220" s="101"/>
+      <c r="D220" s="101"/>
+      <c r="E220" s="101"/>
+      <c r="F220" s="102"/>
     </row>
     <row r="221" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A221" s="27">
         <v>219</v>
       </c>
-      <c r="B221" s="103"/>
-      <c r="C221" s="104"/>
-      <c r="D221" s="104"/>
-      <c r="E221" s="104"/>
-      <c r="F221" s="105"/>
+      <c r="B221" s="100"/>
+      <c r="C221" s="101"/>
+      <c r="D221" s="101"/>
+      <c r="E221" s="101"/>
+      <c r="F221" s="102"/>
     </row>
     <row r="222" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A222" s="24">
@@ -19879,11 +19888,11 @@
       <c r="B222" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="C222" s="118" t="s">
+      <c r="C222" s="85" t="s">
         <v>583</v>
       </c>
-      <c r="D222" s="119"/>
-      <c r="E222" s="120"/>
+      <c r="D222" s="86"/>
+      <c r="E222" s="87"/>
       <c r="F222" s="25" t="s">
         <v>556</v>
       </c>
@@ -19900,7 +19909,7 @@
         <v>719</v>
       </c>
       <c r="E223" s="60" t="s">
-        <v>805</v>
+        <v>869</v>
       </c>
       <c r="F223" s="25" t="s">
         <v>557</v>
@@ -19918,7 +19927,7 @@
         <v>720</v>
       </c>
       <c r="E224" s="60" t="s">
-        <v>806</v>
+        <v>870</v>
       </c>
       <c r="F224" s="25" t="s">
         <v>558</v>
@@ -19938,7 +19947,7 @@
         <v>721</v>
       </c>
       <c r="E225" s="61" t="s">
-        <v>807</v>
+        <v>871</v>
       </c>
       <c r="F225" s="31" t="s">
         <v>559</v>
@@ -19948,18 +19957,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="25">
-    <mergeCell ref="C222:E222"/>
-    <mergeCell ref="C104:E106"/>
-    <mergeCell ref="C113:E114"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C155:E156"/>
-    <mergeCell ref="C158:E158"/>
-    <mergeCell ref="B214:F221"/>
-    <mergeCell ref="B130:F135"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B166:F177"/>
-    <mergeCell ref="B201:F210"/>
-    <mergeCell ref="B199:F199"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H3:K3"/>
@@ -19973,6 +19970,18 @@
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="C51:E53"/>
     <mergeCell ref="C79:E85"/>
+    <mergeCell ref="C222:E222"/>
+    <mergeCell ref="C104:E106"/>
+    <mergeCell ref="C113:E114"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C155:E156"/>
+    <mergeCell ref="C158:E158"/>
+    <mergeCell ref="B214:F221"/>
+    <mergeCell ref="B130:F135"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B166:F177"/>
+    <mergeCell ref="B201:F210"/>
+    <mergeCell ref="B199:F199"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C3 C10 C21 C26 C15 C49 C51 C79 C104 C113 C129 C155 C158 C222">

</xml_diff>